<commit_message>
fix(data): handling missing data at the beginning and at the end of the series
It's only a first step, there is a lot to check and test
</commit_message>
<xml_diff>
--- a/data/MSCI-test-monthly.xlsx
+++ b/data/MSCI-test-monthly.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="328">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">1999-10-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k</t>
   </si>
   <si>
     <t xml:space="preserve">1999-11-30</t>
@@ -1303,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A264" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E231" activeCellId="0" sqref="E231"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1467,13 +1464,10 @@
       <c r="D12" s="1" t="n">
         <v>619.390118</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>3453.111813</v>
@@ -1484,7 +1478,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>3731.987352</v>
@@ -1495,7 +1489,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>3516.599208</v>
@@ -1506,7 +1500,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>3526.214337</v>
@@ -1517,7 +1511,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>3772.658992</v>
@@ -1528,7 +1522,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>3614.228888</v>
@@ -1539,7 +1533,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>3526.456578</v>
@@ -1552,7 +1546,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>3645.845289</v>
@@ -1564,7 +1558,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>3542.467903</v>
@@ -1576,7 +1570,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>3659.163424</v>
@@ -1588,7 +1582,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>3464.49327</v>
@@ -1600,7 +1594,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>3405.299737</v>
@@ -1612,7 +1606,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>3198.647437</v>
@@ -1624,7 +1618,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>3249.513038</v>
@@ -1636,7 +1630,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>3312.625898</v>
@@ -1648,7 +1642,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>3033.040276</v>
@@ -1660,7 +1654,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>2834.396792</v>
@@ -1672,7 +1666,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>3044.611002</v>
@@ -1684,7 +1678,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>3006.795751</v>
@@ -1696,7 +1690,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>2913.015779</v>
@@ -1708,7 +1702,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>2874.656129</v>
@@ -1720,7 +1714,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>2737.232738</v>
@@ -1732,7 +1726,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>2496.400504</v>
@@ -1743,7 +1737,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>2544.47051</v>
@@ -1756,7 +1750,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>2695.385315</v>
@@ -1769,7 +1763,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>2712.658004</v>
@@ -1780,7 +1774,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>2630.770456</v>
@@ -1794,7 +1788,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>2608.413437</v>
@@ -1808,7 +1802,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>2724.270407</v>
@@ -1822,7 +1816,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>2632.751984</v>
@@ -1836,7 +1830,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>2638.854837</v>
@@ -1850,7 +1844,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>2479.285361</v>
@@ -1864,7 +1858,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>2270.613464</v>
@@ -1878,7 +1872,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>2275.334606</v>
@@ -1892,7 +1886,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>2025.606348</v>
@@ -1906,7 +1900,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>2175.474558</v>
@@ -1920,7 +1914,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>2293.254456</v>
@@ -1934,7 +1928,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>2182.570329</v>
@@ -1948,7 +1942,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>2116.623607</v>
@@ -1962,7 +1956,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>2080.382442</v>
@@ -1976,7 +1970,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>2074.666153</v>
@@ -1990,7 +1984,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>2259.956329</v>
@@ -2004,7 +1998,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>2390.220118</v>
@@ -2018,7 +2012,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>2432.4746</v>
@@ -2032,7 +2026,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>2482.327782</v>
@@ -2046,7 +2040,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>2536.553097</v>
@@ -2060,7 +2054,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>2552.643003</v>
@@ -2074,7 +2068,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>2704.633537</v>
@@ -2088,7 +2082,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>2746.463629</v>
@@ -2102,7 +2096,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>2919.44177</v>
@@ -2116,7 +2110,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>2966.931861</v>
@@ -2130,7 +2124,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>3017.675344</v>
@@ -2144,7 +2138,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>2998.82999</v>
@@ -2158,7 +2152,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>2939.075723</v>
@@ -2172,7 +2166,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>2967.884134</v>
@@ -2186,7 +2180,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="1" t="n">
         <v>3030.093073</v>
@@ -2200,7 +2194,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1" t="n">
         <v>2931.964193</v>
@@ -2214,7 +2208,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>2946.022205</v>
@@ -2228,7 +2222,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="1" t="n">
         <v>3002.6955</v>
@@ -2242,7 +2236,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="n">
         <v>3076.904211</v>
@@ -2256,7 +2250,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="n">
         <v>3239.895069</v>
@@ -2270,7 +2264,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>3364.558345</v>
@@ -2284,7 +2278,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="n">
         <v>3289.438908</v>
@@ -2298,7 +2292,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B76" s="1" t="n">
         <v>3395.133482</v>
@@ -2312,7 +2306,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B77" s="1" t="n">
         <v>3330.63462</v>
@@ -2326,7 +2320,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" s="1" t="n">
         <v>3260.390162</v>
@@ -2340,7 +2334,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="n">
         <v>3320.818075</v>
@@ -2354,7 +2348,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1" t="n">
         <v>3351.01918</v>
@@ -2368,7 +2362,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="n">
         <v>3468.822784</v>
@@ -2382,7 +2376,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B82" s="1" t="n">
         <v>3496.581253</v>
@@ -2396,7 +2390,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" s="1" t="n">
         <v>3588.40956</v>
@@ -2410,7 +2404,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="n">
         <v>3502.062889</v>
@@ -2424,7 +2418,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="n">
         <v>3620.657193</v>
@@ -2438,7 +2432,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="n">
         <v>3701.794585</v>
@@ -2452,7 +2446,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1" t="n">
         <v>3867.81377</v>
@@ -2466,7 +2460,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B88" s="1" t="n">
         <v>3863.679046</v>
@@ -2480,7 +2474,7 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="n">
         <v>3950.381312</v>
@@ -2494,7 +2488,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B90" s="1" t="n">
         <v>4072.426018</v>
@@ -2508,7 +2502,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" s="1" t="n">
         <v>3936.963505</v>
@@ -2522,7 +2516,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B92" s="1" t="n">
         <v>3937.43287</v>
@@ -2536,7 +2530,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B93" s="1" t="n">
         <v>3962.860777</v>
@@ -2550,7 +2544,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B94" s="1" t="n">
         <v>4067.753546</v>
@@ -2564,7 +2558,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B95" s="1" t="n">
         <v>4117.42896</v>
@@ -2578,7 +2572,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="1" t="n">
         <v>4269.390748</v>
@@ -2592,7 +2586,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B97" s="1" t="n">
         <v>4376.153465</v>
@@ -2606,7 +2600,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B98" s="1" t="n">
         <v>4466.298194</v>
@@ -2620,7 +2614,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B99" s="1" t="n">
         <v>4519.914584</v>
@@ -2634,7 +2628,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="1" t="n">
         <v>4498.257682</v>
@@ -2648,7 +2642,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="n">
         <v>4582.511727</v>
@@ -2662,7 +2656,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B102" s="1" t="n">
         <v>4787.379529</v>
@@ -2676,7 +2670,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B103" s="1" t="n">
         <v>4926.190984</v>
@@ -2690,7 +2684,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B104" s="1" t="n">
         <v>4889.921852</v>
@@ -2704,7 +2698,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B105" s="1" t="n">
         <v>4782.624196</v>
@@ -2718,7 +2712,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B106" s="1" t="n">
         <v>4781.075029</v>
@@ -2732,7 +2726,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B107" s="1" t="n">
         <v>5010.068913</v>
@@ -2746,7 +2740,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B108" s="1" t="n">
         <v>5164.824547</v>
@@ -2760,7 +2754,7 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B109" s="1" t="n">
         <v>4956.048845</v>
@@ -2774,7 +2768,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B110" s="1" t="n">
         <v>4893.542599</v>
@@ -2788,7 +2782,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B111" s="1" t="n">
         <v>4520.672214</v>
@@ -2802,7 +2796,7 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B112" s="1" t="n">
         <v>4496.69501</v>
@@ -2816,7 +2810,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B113" s="1" t="n">
         <v>4455.80466</v>
@@ -2830,7 +2824,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B114" s="1" t="n">
         <v>4693.577317</v>
@@ -2844,7 +2838,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B115" s="1" t="n">
         <v>4770.995512</v>
@@ -2858,7 +2852,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B116" s="1" t="n">
         <v>4392.17244</v>
@@ -2872,7 +2866,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B117" s="1" t="n">
         <v>4285.968826</v>
@@ -2886,7 +2880,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B118" s="1" t="n">
         <v>4227.702323</v>
@@ -2900,7 +2894,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B119" s="1" t="n">
         <v>3726.687575</v>
@@ -2914,7 +2908,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B120" s="1" t="n">
         <v>3021.073597</v>
@@ -2928,7 +2922,7 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B121" s="1" t="n">
         <v>2827.607531</v>
@@ -2942,7 +2936,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B122" s="1" t="n">
         <v>2919.782614</v>
@@ -2956,7 +2950,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B123" s="1" t="n">
         <v>2664.847172</v>
@@ -2970,7 +2964,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B124" s="1" t="n">
         <v>2393.873995</v>
@@ -2984,7 +2978,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B125" s="1" t="n">
         <v>2575.816373</v>
@@ -2998,7 +2992,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B126" s="1" t="n">
         <v>2867.371642</v>
@@ -3012,7 +3006,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B127" s="1" t="n">
         <v>3130.78568</v>
@@ -3026,7 +3020,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B128" s="1" t="n">
         <v>3117.982151</v>
@@ -3040,7 +3034,7 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B129" s="1" t="n">
         <v>3383.009336</v>
@@ -3054,7 +3048,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B130" s="1" t="n">
         <v>3524.075058</v>
@@ -3068,7 +3062,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B131" s="1" t="n">
         <v>3665.755558</v>
@@ -3082,7 +3076,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B132" s="1" t="n">
         <v>3601.322067</v>
@@ -3096,7 +3090,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B133" s="1" t="n">
         <v>3750.306086</v>
@@ -3110,7 +3104,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B134" s="1" t="n">
         <v>3818.859038</v>
@@ -3124,7 +3118,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B135" s="1" t="n">
         <v>3661.751978</v>
@@ -3138,7 +3132,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B136" s="1" t="n">
         <v>3714.830292</v>
@@ -3152,7 +3146,7 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B137" s="1" t="n">
         <v>3946.960009</v>
@@ -3166,7 +3160,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B138" s="1" t="n">
         <v>3949.717839</v>
@@ -3180,7 +3174,7 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B139" s="1" t="n">
         <v>3575.136513</v>
@@ -3194,7 +3188,7 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B140" s="1" t="n">
         <v>3453.891084</v>
@@ -3208,7 +3202,7 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B141" s="1" t="n">
         <v>3734.815772</v>
@@ -3222,7 +3216,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B142" s="1" t="n">
         <v>3596.902173</v>
@@ -3236,7 +3230,7 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B143" s="1" t="n">
         <v>3933.681227</v>
@@ -3250,7 +3244,7 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B144" s="1" t="n">
         <v>4081.18627</v>
@@ -3264,7 +3258,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B145" s="1" t="n">
         <v>3994.994271</v>
@@ -3278,7 +3272,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B146" s="1" t="n">
         <v>4290.045368</v>
@@ -3292,7 +3286,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B147" s="1" t="n">
         <v>4387.969544</v>
@@ -3306,7 +3300,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B148" s="1" t="n">
         <v>4543.546134</v>
@@ -3320,7 +3314,7 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B149" s="1" t="n">
         <v>4500.825242</v>
@@ -3334,7 +3328,7 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B150" s="1" t="n">
         <v>4694.883908</v>
@@ -3348,7 +3342,7 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B151" s="1" t="n">
         <v>4602.240757</v>
@@ -3362,7 +3356,7 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B152" s="1" t="n">
         <v>4531.207531</v>
@@ -3376,7 +3370,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B153" s="1" t="n">
         <v>4450.249251</v>
@@ -3390,7 +3384,7 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B154" s="1" t="n">
         <v>4138.562322</v>
@@ -3404,7 +3398,7 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B155" s="1" t="n">
         <v>3782.757039</v>
@@ -3418,7 +3412,7 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B156" s="1" t="n">
         <v>4175.102956</v>
@@ -3432,7 +3426,7 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B157" s="1" t="n">
         <v>4075.560085</v>
@@ -3446,7 +3440,7 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B158" s="1" t="n">
         <v>4074.833677</v>
@@ -3460,7 +3454,7 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B159" s="1" t="n">
         <v>4280.520734</v>
@@ -3474,7 +3468,7 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B160" s="1" t="n">
         <v>4491.978708</v>
@@ -3488,7 +3482,7 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B161" s="1" t="n">
         <v>4552.201557</v>
@@ -3502,7 +3496,7 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B162" s="1" t="n">
         <v>4503.679588</v>
@@ -3516,7 +3510,7 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B163" s="1" t="n">
         <v>4119.206386</v>
@@ -3530,7 +3524,7 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B164" s="1" t="n">
         <v>4331.155403</v>
@@ -3544,7 +3538,7 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B165" s="1" t="n">
         <v>4388.035805</v>
@@ -3558,7 +3552,7 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B166" s="1" t="n">
         <v>4501.500939</v>
@@ -3572,7 +3566,7 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B167" s="1" t="n">
         <v>4627.184251</v>
@@ -3586,7 +3580,7 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B168" s="1" t="n">
         <v>4597.231193</v>
@@ -3600,7 +3594,7 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B169" s="1" t="n">
         <v>4658.581487</v>
@@ -3614,7 +3608,7 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B170" s="1" t="n">
         <v>4748.698511</v>
@@ -3628,7 +3622,7 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B171" s="1" t="n">
         <v>4992.061167</v>
@@ -3642,7 +3636,7 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B172" s="1" t="n">
         <v>5002.798508</v>
@@ -3656,7 +3650,7 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B173" s="1" t="n">
         <v>5122.563061</v>
@@ -3670,7 +3664,7 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B174" s="1" t="n">
         <v>5287.524128</v>
@@ -3684,7 +3678,7 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B175" s="1" t="n">
         <v>5294.214565</v>
@@ -3698,7 +3692,7 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B176" s="1" t="n">
         <v>5165.877084</v>
@@ -3712,7 +3706,7 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B177" s="1" t="n">
         <v>5439.34652</v>
@@ -3726,7 +3720,7 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B178" s="1" t="n">
         <v>5325.887115</v>
@@ -3740,7 +3734,7 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B179" s="1" t="n">
         <v>5594.335573</v>
@@ -3754,7 +3748,7 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B180" s="1" t="n">
         <v>5814.648991</v>
@@ -3768,7 +3762,7 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B181" s="1" t="n">
         <v>5920.682817</v>
@@ -3782,7 +3776,7 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B182" s="1" t="n">
         <v>6048.181012</v>
@@ -3796,7 +3790,7 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B183" s="1" t="n">
         <v>5825.526876</v>
@@ -3810,7 +3804,7 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B184" s="1" t="n">
         <v>6120.253606</v>
@@ -3824,7 +3818,7 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B185" s="1" t="n">
         <v>6132.591574</v>
@@ -3838,7 +3832,7 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B186" s="1" t="n">
         <v>6198.797954</v>
@@ -3852,7 +3846,7 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B187" s="1" t="n">
         <v>6326.600987</v>
@@ -3866,7 +3860,7 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B188" s="1" t="n">
         <v>6442.500674</v>
@@ -3880,7 +3874,7 @@
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B189" s="1" t="n">
         <v>6341.234415</v>
@@ -3894,7 +3888,7 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B190" s="1" t="n">
         <v>6483.570232</v>
@@ -3908,7 +3902,7 @@
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B191" s="1" t="n">
         <v>6310.268156</v>
@@ -3922,7 +3916,7 @@
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B192" s="1" t="n">
         <v>6352.598337</v>
@@ -3936,7 +3930,7 @@
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B193" s="1" t="n">
         <v>6482.900453</v>
@@ -3950,7 +3944,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B194" s="1" t="n">
         <v>6381.054489</v>
@@ -3964,7 +3958,7 @@
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B195" s="1" t="n">
         <v>6266.933709</v>
@@ -3978,7 +3972,7 @@
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B196" s="1" t="n">
         <v>6637.222188</v>
@@ -3992,7 +3986,7 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B197" s="1" t="n">
         <v>6537.618526</v>
@@ -4006,7 +4000,7 @@
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B198" s="1" t="n">
         <v>6694.313819</v>
@@ -4020,7 +4014,7 @@
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B199" s="1" t="n">
         <v>6723.059942</v>
@@ -4034,7 +4028,7 @@
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B200" s="1" t="n">
         <v>6569.46635</v>
@@ -4048,7 +4042,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B201" s="1" t="n">
         <v>6689.575637</v>
@@ -4062,7 +4056,7 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B202" s="1" t="n">
         <v>6249.64635</v>
@@ -4076,7 +4070,7 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B203" s="1" t="n">
         <v>6021.954302</v>
@@ -4090,7 +4084,7 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B204" s="1" t="n">
         <v>6500.909759</v>
@@ -4104,7 +4098,7 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B205" s="1" t="n">
         <v>6471.71718</v>
@@ -4118,7 +4112,7 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B206" s="1" t="n">
         <v>6360.574954</v>
@@ -4132,7 +4126,7 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B207" s="1" t="n">
         <v>5981.67427</v>
@@ -4146,7 +4140,7 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B208" s="1" t="n">
         <v>5940.800331</v>
@@ -4160,7 +4154,7 @@
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B209" s="1" t="n">
         <v>6348.294514</v>
@@ -4174,7 +4168,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B210" s="1" t="n">
         <v>6452.776567</v>
@@ -4188,7 +4182,7 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B211" s="1" t="n">
         <v>6494.942746</v>
@@ -4202,7 +4196,7 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B212" s="1" t="n">
         <v>6425.279863</v>
@@ -4216,7 +4210,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B213" s="1" t="n">
         <v>6698.465937</v>
@@ -4230,7 +4224,7 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B214" s="1" t="n">
         <v>6707.420309</v>
@@ -4244,7 +4238,7 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B215" s="1" t="n">
         <v>6746.076641</v>
@@ -4258,7 +4252,7 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B216" s="1" t="n">
         <v>6617.258395</v>
@@ -4272,7 +4266,7 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B217" s="1" t="n">
         <v>6716.016518</v>
@@ -4286,7 +4280,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B218" s="1" t="n">
         <v>6879.162363</v>
@@ -4300,7 +4294,7 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B219" s="1" t="n">
         <v>7046.796149</v>
@@ -4314,7 +4308,7 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B220" s="1" t="n">
         <v>7245.762912</v>
@@ -4328,7 +4322,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B221" s="1" t="n">
         <v>7328.13507</v>
@@ -4342,7 +4336,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B222" s="1" t="n">
         <v>7440.259608</v>
@@ -4356,7 +4350,7 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B223" s="1" t="n">
         <v>7604.861196</v>
@@ -4370,7 +4364,7 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B224" s="1" t="n">
         <v>7637.015307</v>
@@ -4384,7 +4378,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B225" s="1" t="n">
         <v>7822.146969</v>
@@ -4398,7 +4392,7 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B226" s="1" t="n">
         <v>7837.107664</v>
@@ -4412,7 +4406,7 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B227" s="1" t="n">
         <v>8016.091279</v>
@@ -4426,7 +4420,7 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B228" s="1" t="n">
         <v>8169.600974</v>
@@ -4440,7 +4434,7 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B229" s="1" t="n">
         <v>8350.801848</v>
@@ -4454,7 +4448,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B230" s="1" t="n">
         <v>8466.344501</v>
@@ -4468,7 +4462,7 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B231" s="1" t="n">
         <v>8915.277691</v>
@@ -4482,7 +4476,7 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B232" s="1" t="n">
         <v>8549.698834</v>
@@ -4496,7 +4490,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B233" s="1" t="n">
         <v>8368.878782</v>
@@ -4510,7 +4504,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B234" s="1" t="n">
         <v>8470.212767</v>
@@ -4524,7 +4518,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B235" s="1" t="n">
         <v>8531.326869</v>
@@ -4538,7 +4532,7 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B236" s="1" t="n">
         <v>8530.353984</v>
@@ -4552,7 +4546,7 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B237" s="1" t="n">
         <v>8798.941068</v>
@@ -4566,7 +4560,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B238" s="1" t="n">
         <v>8911.933486</v>
@@ -4580,7 +4574,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B239" s="1" t="n">
         <v>8965.287627</v>
@@ -4594,7 +4588,7 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B240" s="1" t="n">
         <v>8309.110332</v>
@@ -4608,7 +4602,7 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B241" s="1" t="n">
         <v>8407.844611</v>
@@ -4622,7 +4616,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B242" s="1" t="n">
         <v>7771.710261</v>
@@ -4636,7 +4630,7 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B243" s="1" t="n">
         <v>8379.028953</v>
@@ -4650,7 +4644,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B244" s="1" t="n">
         <v>8635.203361</v>
@@ -4664,7 +4658,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B245" s="1" t="n">
         <v>8754.488883</v>
@@ -4678,7 +4672,7 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B246" s="1" t="n">
         <v>9069.951224</v>
@@ -4692,7 +4686,7 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B247" s="1" t="n">
         <v>8554.772217</v>
@@ -4706,7 +4700,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B248" s="1" t="n">
         <v>9122.090094</v>
@@ -4720,7 +4714,7 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B249" s="1" t="n">
         <v>9169.81569</v>
@@ -4734,7 +4728,7 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B250" s="1" t="n">
         <v>8986.643663</v>
@@ -4748,7 +4742,7 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B251" s="1" t="n">
         <v>9182.16764</v>
@@ -4762,7 +4756,7 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B252" s="1" t="n">
         <v>9418.381319</v>
@@ -4776,7 +4770,7 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B253" s="1" t="n">
         <v>9685.175388</v>
@@ -4790,7 +4784,7 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B254" s="1" t="n">
         <v>9979.03366</v>
@@ -4804,7 +4798,7 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B255" s="1" t="n">
         <v>9921.108777</v>
@@ -4818,7 +4812,7 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B256" s="1" t="n">
         <v>9086.788157</v>
@@ -4832,7 +4826,7 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B257" s="1" t="n">
         <v>7890.18073</v>
@@ -4846,7 +4840,7 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B258" s="1" t="n">
         <v>8756.464871</v>
@@ -4860,7 +4854,7 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B259" s="1" t="n">
         <v>9185.249174</v>
@@ -4874,7 +4868,7 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B260" s="1" t="n">
         <v>9432.107145</v>
@@ -4888,7 +4882,7 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B261" s="1" t="n">
         <v>9886.493432</v>
@@ -4902,7 +4896,7 @@
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B262" s="1" t="n">
         <v>10550.971824</v>
@@ -4916,7 +4910,7 @@
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B263" s="1" t="n">
         <v>10191.07874</v>
@@ -4930,7 +4924,7 @@
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B264" s="1" t="n">
         <v>9881.075667</v>
@@ -4944,7 +4938,7 @@
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B265" s="1" t="n">
         <v>11148.599773</v>
@@ -4958,7 +4952,7 @@
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B266" s="1" t="n">
         <v>11625.198749</v>
@@ -4972,7 +4966,7 @@
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B267" s="1" t="n">
         <v>11512.425105</v>
@@ -4986,7 +4980,7 @@
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B268" s="1" t="n">
         <v>11811.310416</v>
@@ -5000,7 +4994,7 @@
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B269" s="1" t="n">
         <v>12211.116272</v>
@@ -5014,7 +5008,7 @@
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B270" s="1" t="n">
         <v>12784.973299</v>
@@ -5028,7 +5022,7 @@
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B271" s="1" t="n">
         <v>12976.577906</v>
@@ -5042,7 +5036,7 @@
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B272" s="1" t="n">
         <v>13174.250989</v>
@@ -5056,7 +5050,7 @@
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B273" s="1" t="n">
         <v>13413.449833</v>
@@ -5070,7 +5064,7 @@
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B274" s="1" t="n">
         <v>13751.460508</v>
@@ -5084,7 +5078,7 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B275" s="1" t="n">
         <v>13186.526695</v>
@@ -5098,7 +5092,7 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B276" s="1" t="n">
         <v>13936.992021</v>
@@ -5112,7 +5106,7 @@
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B277" s="1" t="n">
         <v>13636.233449</v>
@@ -5126,7 +5120,7 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B278" s="1" t="n">
         <v>14223.136794</v>
@@ -5140,7 +5134,7 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B279" s="1" t="n">
         <v>13473.4354</v>
@@ -5154,7 +5148,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B280" s="1" t="n">
         <v>13137.03442</v>
@@ -5168,7 +5162,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B281" s="1" t="n">
         <v>13505.741311</v>
@@ -5182,7 +5176,7 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B282" s="1" t="n">
         <v>12389.188861</v>
@@ -5196,7 +5190,7 @@
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B283" s="1" t="n">
         <v>12408.089771</v>
@@ -5210,7 +5204,7 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B284" s="1" t="n">
         <v>11337.723549</v>
@@ -5224,7 +5218,7 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B285" s="1" t="n">
         <v>12241.139674</v>
@@ -5238,7 +5232,7 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B286" s="1" t="n">
         <v>11734.160889</v>
@@ -5252,7 +5246,7 @@
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B287" s="1" t="n">
         <v>10648.162536</v>
@@ -5266,373 +5260,475 @@
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B288" s="1" t="n">
         <v>11415.734483</v>
       </c>
+      <c r="C288" s="1" t="n">
+        <v>1300.54199</v>
+      </c>
       <c r="D288" s="1" t="n">
         <v>2175.980513</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B289" s="1" t="n">
         <v>12215.105868</v>
       </c>
+      <c r="C289" s="1" t="n">
+        <v>1402.013192</v>
+      </c>
       <c r="D289" s="1" t="n">
         <v>2342.569892</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B290" s="1" t="n">
         <v>11700.992418</v>
       </c>
+      <c r="C290" s="1" t="n">
+        <v>1347.399869</v>
+      </c>
       <c r="D290" s="1" t="n">
         <v>2253.545483</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B291" s="1" t="n">
         <v>12532.085435</v>
       </c>
+      <c r="C291" s="1" t="n">
+        <v>1444.315908</v>
+      </c>
       <c r="D291" s="1" t="n">
         <v>2420.084533</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B292" s="1" t="n">
         <v>12235.685754</v>
       </c>
+      <c r="C292" s="1" t="n">
+        <v>1403.429303</v>
+      </c>
       <c r="D292" s="1" t="n">
         <v>2353.661544</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B293" s="1" t="n">
         <v>12622.659609</v>
       </c>
+      <c r="C293" s="1" t="n">
+        <v>1447.674908</v>
+      </c>
       <c r="D293" s="1" t="n">
         <v>2413.189052</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B294" s="1" t="n">
         <v>12850.378508</v>
       </c>
+      <c r="C294" s="1" t="n">
+        <v>1469.169928</v>
+      </c>
       <c r="D294" s="1" t="n">
         <v>2445.046213</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B295" s="1" t="n">
         <v>12731.907782</v>
       </c>
+      <c r="C295" s="1" t="n">
+        <v>1454.481784</v>
+      </c>
       <c r="D295" s="1" t="n">
         <v>2417.27619</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B296" s="1" t="n">
         <v>13506.744492</v>
       </c>
+      <c r="C296" s="1" t="n">
+        <v>1539.573475</v>
+      </c>
       <c r="D296" s="1" t="n">
         <v>2559.355543</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B297" s="1" t="n">
         <v>13963.885805</v>
       </c>
+      <c r="C297" s="1" t="n">
+        <v>1596.391861</v>
+      </c>
       <c r="D297" s="1" t="n">
         <v>2657.986157</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B298" s="1" t="n">
         <v>13636.081474</v>
       </c>
+      <c r="C298" s="1" t="n">
+        <v>1552.416902</v>
+      </c>
       <c r="D298" s="1" t="n">
         <v>2582.717382</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B299" s="1" t="n">
         <v>13052.604114</v>
       </c>
+      <c r="C299" s="1" t="n">
+        <v>1488.773934</v>
+      </c>
       <c r="D299" s="1" t="n">
         <v>2474.944252</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B300" s="1" t="n">
         <v>12676.970282</v>
       </c>
+      <c r="C300" s="1" t="n">
+        <v>1444.344327</v>
+      </c>
       <c r="D300" s="1" t="n">
         <v>2393.03758</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B301" s="1" t="n">
         <v>13871.961001</v>
       </c>
+      <c r="C301" s="1" t="n">
+        <v>1578.338665</v>
+      </c>
       <c r="D301" s="1" t="n">
         <v>2615.355825</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B302" s="1" t="n">
         <v>14557.826422</v>
       </c>
+      <c r="C302" s="1" t="n">
+        <v>1654.705023</v>
+      </c>
       <c r="D302" s="1" t="n">
         <v>2753.489562</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B303" s="1" t="n">
         <v>14735.888914</v>
       </c>
+      <c r="C303" s="1" t="n">
+        <v>1664.763092</v>
+      </c>
       <c r="D303" s="1" t="n">
         <v>2760.285276</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B304" s="1" t="n">
         <v>15366.381971</v>
       </c>
+      <c r="C304" s="1" t="n">
+        <v>1736.815265</v>
+      </c>
       <c r="D304" s="1" t="n">
         <v>2876.617573</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B305" s="1" t="n">
         <v>15868.8896</v>
       </c>
+      <c r="C305" s="1" t="n">
+        <v>1792.3067</v>
+      </c>
       <c r="D305" s="1" t="n">
         <v>2969.190277</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B306" s="1" t="n">
         <v>15286.59151</v>
       </c>
+      <c r="C306" s="1" t="n">
+        <v>1733.93893</v>
+      </c>
       <c r="D306" s="1" t="n">
         <v>2869.658728</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B307" s="1" t="n">
         <v>15979.455491</v>
       </c>
+      <c r="C307" s="1" t="n">
+        <v>1805.457166</v>
+      </c>
       <c r="D307" s="1" t="n">
         <v>2987.735697</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B308" s="1" t="n">
         <v>16309.886618</v>
       </c>
+      <c r="C308" s="1" t="n">
+        <v>1846.320461</v>
+      </c>
       <c r="D308" s="1" t="n">
         <v>3044.186119</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B309" s="1" t="n">
         <v>16601.012475</v>
       </c>
+      <c r="C309" s="1" t="n">
+        <v>1876.606339</v>
+      </c>
       <c r="D309" s="1" t="n">
         <v>3107.654519</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B310" s="1" t="n">
         <v>17045.470265</v>
       </c>
+      <c r="C310" s="1" t="n">
+        <v>1924.907114</v>
+      </c>
       <c r="D310" s="1" t="n">
         <v>3181.292958</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B311" s="1" t="n">
         <v>17364.011736</v>
       </c>
+      <c r="C311" s="1" t="n">
+        <v>1970.352877</v>
+      </c>
       <c r="D311" s="1" t="n">
         <v>3255.7756</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B312" s="1" t="n">
         <v>17023.445476</v>
       </c>
+      <c r="C312" s="1" t="n">
+        <v>1926.776187</v>
+      </c>
       <c r="D312" s="1" t="n">
         <v>3181.390406</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B313" s="1" t="n">
         <v>17810.63517</v>
       </c>
+      <c r="C313" s="1" t="n">
+        <v>1999.474831</v>
+      </c>
       <c r="D313" s="1" t="n">
         <v>3306.465261</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B314" s="1" t="n">
         <v>17352.115351</v>
       </c>
+      <c r="C314" s="1" t="n">
+        <v>1952.803514</v>
+      </c>
       <c r="D314" s="1" t="n">
         <v>3218.643567</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B315" s="1" t="n">
         <v>17968.349835</v>
       </c>
+      <c r="C315" s="1" t="n">
+        <v>2018.786618</v>
+      </c>
       <c r="D315" s="1" t="n">
         <v>3324.731672</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B316" s="1" t="n">
         <v>17844.251038</v>
       </c>
+      <c r="C316" s="1" t="n">
+        <v>2007.191047</v>
+      </c>
       <c r="D316" s="1" t="n">
         <v>3296.400292</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B317" s="1" t="n">
         <v>17059.748793</v>
       </c>
+      <c r="C317" s="1" t="n">
+        <v>1928.980371</v>
+      </c>
       <c r="D317" s="1" t="n">
         <v>3170.354511</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B318" s="1" t="n">
         <v>17219.319838</v>
       </c>
+      <c r="C318" s="1" t="n">
+        <v>1947.837353</v>
+      </c>
       <c r="D318" s="1" t="n">
         <v>3201.495285</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B319" s="1" t="n">
         <v>18250.358313</v>
       </c>
+      <c r="C319" s="1" t="n">
+        <v>2061.073367</v>
+      </c>
       <c r="D319" s="1" t="n">
         <v>3388.827013</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B320" s="1" t="n">
         <v>19044.007434</v>
       </c>
+      <c r="C320" s="1" t="n">
+        <v>2154.502262</v>
+      </c>
       <c r="D320" s="1" t="n">
         <v>3543.895587</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B321" s="1" t="n">
         <v>19293.050929</v>
+      </c>
+      <c r="C321" s="1" t="n">
+        <v>2184.265977</v>
       </c>
       <c r="D321" s="1" t="n">
         <v>3591.95791</v>

</xml_diff>

<commit_message>
fix(data): robust - I hope -  leftover window calculation per column
Calculate leftover window size and start date independently for each
column
based on the number of valid periods after the last complete window.
Ensure
output includes annualized return, starting date, and period count for
each
column. Prevents misleading results when trailing data is missing.
</commit_message>
<xml_diff>
--- a/data/MSCI-test-monthly.xlsx
+++ b/data/MSCI-test-monthly.xlsx
@@ -1300,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A266" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F280" activeCellId="0" sqref="F280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5195,9 +5195,6 @@
       <c r="B283" s="1" t="n">
         <v>12408.089771</v>
       </c>
-      <c r="C283" s="1" t="n">
-        <v>1434.750855</v>
-      </c>
       <c r="D283" s="1" t="n">
         <v>2398.255114</v>
       </c>
@@ -5209,9 +5206,6 @@
       <c r="B284" s="1" t="n">
         <v>11337.723549</v>
       </c>
-      <c r="C284" s="1" t="n">
-        <v>1314.397654</v>
-      </c>
       <c r="D284" s="1" t="n">
         <v>2192.381148</v>
       </c>
@@ -5223,9 +5217,6 @@
       <c r="B285" s="1" t="n">
         <v>12241.139674</v>
       </c>
-      <c r="C285" s="1" t="n">
-        <v>1406.650278</v>
-      </c>
       <c r="D285" s="1" t="n">
         <v>2349.777329</v>
       </c>
@@ -5237,9 +5228,6 @@
       <c r="B286" s="1" t="n">
         <v>11734.160889</v>
       </c>
-      <c r="C286" s="1" t="n">
-        <v>1355.412966</v>
-      </c>
       <c r="D286" s="1" t="n">
         <v>2267.263828</v>
       </c>
@@ -5251,9 +5239,6 @@
       <c r="B287" s="1" t="n">
         <v>10648.162536</v>
       </c>
-      <c r="C287" s="1" t="n">
-        <v>1226.229237</v>
-      </c>
       <c r="D287" s="1" t="n">
         <v>2049.383435</v>
       </c>
@@ -5265,9 +5250,6 @@
       <c r="B288" s="1" t="n">
         <v>11415.734483</v>
       </c>
-      <c r="C288" s="1" t="n">
-        <v>1300.54199</v>
-      </c>
       <c r="D288" s="1" t="n">
         <v>2175.980513</v>
       </c>
@@ -5279,9 +5261,6 @@
       <c r="B289" s="1" t="n">
         <v>12215.105868</v>
       </c>
-      <c r="C289" s="1" t="n">
-        <v>1402.013192</v>
-      </c>
       <c r="D289" s="1" t="n">
         <v>2342.569892</v>
       </c>
@@ -5293,9 +5272,6 @@
       <c r="B290" s="1" t="n">
         <v>11700.992418</v>
       </c>
-      <c r="C290" s="1" t="n">
-        <v>1347.399869</v>
-      </c>
       <c r="D290" s="1" t="n">
         <v>2253.545483</v>
       </c>
@@ -5307,9 +5283,6 @@
       <c r="B291" s="1" t="n">
         <v>12532.085435</v>
       </c>
-      <c r="C291" s="1" t="n">
-        <v>1444.315908</v>
-      </c>
       <c r="D291" s="1" t="n">
         <v>2420.084533</v>
       </c>
@@ -5321,9 +5294,6 @@
       <c r="B292" s="1" t="n">
         <v>12235.685754</v>
       </c>
-      <c r="C292" s="1" t="n">
-        <v>1403.429303</v>
-      </c>
       <c r="D292" s="1" t="n">
         <v>2353.661544</v>
       </c>
@@ -5335,9 +5305,6 @@
       <c r="B293" s="1" t="n">
         <v>12622.659609</v>
       </c>
-      <c r="C293" s="1" t="n">
-        <v>1447.674908</v>
-      </c>
       <c r="D293" s="1" t="n">
         <v>2413.189052</v>
       </c>
@@ -5349,9 +5316,6 @@
       <c r="B294" s="1" t="n">
         <v>12850.378508</v>
       </c>
-      <c r="C294" s="1" t="n">
-        <v>1469.169928</v>
-      </c>
       <c r="D294" s="1" t="n">
         <v>2445.046213</v>
       </c>
@@ -5363,9 +5327,6 @@
       <c r="B295" s="1" t="n">
         <v>12731.907782</v>
       </c>
-      <c r="C295" s="1" t="n">
-        <v>1454.481784</v>
-      </c>
       <c r="D295" s="1" t="n">
         <v>2417.27619</v>
       </c>
@@ -5377,9 +5338,6 @@
       <c r="B296" s="1" t="n">
         <v>13506.744492</v>
       </c>
-      <c r="C296" s="1" t="n">
-        <v>1539.573475</v>
-      </c>
       <c r="D296" s="1" t="n">
         <v>2559.355543</v>
       </c>
@@ -5391,9 +5349,6 @@
       <c r="B297" s="1" t="n">
         <v>13963.885805</v>
       </c>
-      <c r="C297" s="1" t="n">
-        <v>1596.391861</v>
-      </c>
       <c r="D297" s="1" t="n">
         <v>2657.986157</v>
       </c>
@@ -5405,9 +5360,6 @@
       <c r="B298" s="1" t="n">
         <v>13636.081474</v>
       </c>
-      <c r="C298" s="1" t="n">
-        <v>1552.416902</v>
-      </c>
       <c r="D298" s="1" t="n">
         <v>2582.717382</v>
       </c>
@@ -5419,9 +5371,6 @@
       <c r="B299" s="1" t="n">
         <v>13052.604114</v>
       </c>
-      <c r="C299" s="1" t="n">
-        <v>1488.773934</v>
-      </c>
       <c r="D299" s="1" t="n">
         <v>2474.944252</v>
       </c>
@@ -5433,9 +5382,6 @@
       <c r="B300" s="1" t="n">
         <v>12676.970282</v>
       </c>
-      <c r="C300" s="1" t="n">
-        <v>1444.344327</v>
-      </c>
       <c r="D300" s="1" t="n">
         <v>2393.03758</v>
       </c>
@@ -5447,9 +5393,6 @@
       <c r="B301" s="1" t="n">
         <v>13871.961001</v>
       </c>
-      <c r="C301" s="1" t="n">
-        <v>1578.338665</v>
-      </c>
       <c r="D301" s="1" t="n">
         <v>2615.355825</v>
       </c>
@@ -5461,9 +5404,6 @@
       <c r="B302" s="1" t="n">
         <v>14557.826422</v>
       </c>
-      <c r="C302" s="1" t="n">
-        <v>1654.705023</v>
-      </c>
       <c r="D302" s="1" t="n">
         <v>2753.489562</v>
       </c>
@@ -5475,9 +5415,6 @@
       <c r="B303" s="1" t="n">
         <v>14735.888914</v>
       </c>
-      <c r="C303" s="1" t="n">
-        <v>1664.763092</v>
-      </c>
       <c r="D303" s="1" t="n">
         <v>2760.285276</v>
       </c>
@@ -5489,9 +5426,6 @@
       <c r="B304" s="1" t="n">
         <v>15366.381971</v>
       </c>
-      <c r="C304" s="1" t="n">
-        <v>1736.815265</v>
-      </c>
       <c r="D304" s="1" t="n">
         <v>2876.617573</v>
       </c>
@@ -5503,9 +5437,6 @@
       <c r="B305" s="1" t="n">
         <v>15868.8896</v>
       </c>
-      <c r="C305" s="1" t="n">
-        <v>1792.3067</v>
-      </c>
       <c r="D305" s="1" t="n">
         <v>2969.190277</v>
       </c>
@@ -5517,9 +5448,6 @@
       <c r="B306" s="1" t="n">
         <v>15286.59151</v>
       </c>
-      <c r="C306" s="1" t="n">
-        <v>1733.93893</v>
-      </c>
       <c r="D306" s="1" t="n">
         <v>2869.658728</v>
       </c>
@@ -5531,9 +5459,6 @@
       <c r="B307" s="1" t="n">
         <v>15979.455491</v>
       </c>
-      <c r="C307" s="1" t="n">
-        <v>1805.457166</v>
-      </c>
       <c r="D307" s="1" t="n">
         <v>2987.735697</v>
       </c>
@@ -5545,9 +5470,6 @@
       <c r="B308" s="1" t="n">
         <v>16309.886618</v>
       </c>
-      <c r="C308" s="1" t="n">
-        <v>1846.320461</v>
-      </c>
       <c r="D308" s="1" t="n">
         <v>3044.186119</v>
       </c>
@@ -5559,9 +5481,6 @@
       <c r="B309" s="1" t="n">
         <v>16601.012475</v>
       </c>
-      <c r="C309" s="1" t="n">
-        <v>1876.606339</v>
-      </c>
       <c r="D309" s="1" t="n">
         <v>3107.654519</v>
       </c>
@@ -5573,9 +5492,6 @@
       <c r="B310" s="1" t="n">
         <v>17045.470265</v>
       </c>
-      <c r="C310" s="1" t="n">
-        <v>1924.907114</v>
-      </c>
       <c r="D310" s="1" t="n">
         <v>3181.292958</v>
       </c>
@@ -5587,9 +5503,6 @@
       <c r="B311" s="1" t="n">
         <v>17364.011736</v>
       </c>
-      <c r="C311" s="1" t="n">
-        <v>1970.352877</v>
-      </c>
       <c r="D311" s="1" t="n">
         <v>3255.7756</v>
       </c>
@@ -5601,9 +5514,6 @@
       <c r="B312" s="1" t="n">
         <v>17023.445476</v>
       </c>
-      <c r="C312" s="1" t="n">
-        <v>1926.776187</v>
-      </c>
       <c r="D312" s="1" t="n">
         <v>3181.390406</v>
       </c>
@@ -5615,9 +5525,6 @@
       <c r="B313" s="1" t="n">
         <v>17810.63517</v>
       </c>
-      <c r="C313" s="1" t="n">
-        <v>1999.474831</v>
-      </c>
       <c r="D313" s="1" t="n">
         <v>3306.465261</v>
       </c>
@@ -5629,9 +5536,6 @@
       <c r="B314" s="1" t="n">
         <v>17352.115351</v>
       </c>
-      <c r="C314" s="1" t="n">
-        <v>1952.803514</v>
-      </c>
       <c r="D314" s="1" t="n">
         <v>3218.643567</v>
       </c>
@@ -5643,9 +5547,6 @@
       <c r="B315" s="1" t="n">
         <v>17968.349835</v>
       </c>
-      <c r="C315" s="1" t="n">
-        <v>2018.786618</v>
-      </c>
       <c r="D315" s="1" t="n">
         <v>3324.731672</v>
       </c>
@@ -5657,9 +5558,6 @@
       <c r="B316" s="1" t="n">
         <v>17844.251038</v>
       </c>
-      <c r="C316" s="1" t="n">
-        <v>2007.191047</v>
-      </c>
       <c r="D316" s="1" t="n">
         <v>3296.400292</v>
       </c>
@@ -5671,9 +5569,6 @@
       <c r="B317" s="1" t="n">
         <v>17059.748793</v>
       </c>
-      <c r="C317" s="1" t="n">
-        <v>1928.980371</v>
-      </c>
       <c r="D317" s="1" t="n">
         <v>3170.354511</v>
       </c>
@@ -5685,9 +5580,6 @@
       <c r="B318" s="1" t="n">
         <v>17219.319838</v>
       </c>
-      <c r="C318" s="1" t="n">
-        <v>1947.837353</v>
-      </c>
       <c r="D318" s="1" t="n">
         <v>3201.495285</v>
       </c>
@@ -5699,9 +5591,6 @@
       <c r="B319" s="1" t="n">
         <v>18250.358313</v>
       </c>
-      <c r="C319" s="1" t="n">
-        <v>2061.073367</v>
-      </c>
       <c r="D319" s="1" t="n">
         <v>3388.827013</v>
       </c>
@@ -5713,9 +5602,6 @@
       <c r="B320" s="1" t="n">
         <v>19044.007434</v>
       </c>
-      <c r="C320" s="1" t="n">
-        <v>2154.502262</v>
-      </c>
       <c r="D320" s="1" t="n">
         <v>3543.895587</v>
       </c>
@@ -5726,9 +5612,6 @@
       </c>
       <c r="B321" s="1" t="n">
         <v>19293.050929</v>
-      </c>
-      <c r="C321" s="1" t="n">
-        <v>2184.265977</v>
       </c>
       <c r="D321" s="1" t="n">
         <v>3591.95791</v>

</xml_diff>

<commit_message>
feat(firestarter): added argument --config. Played with the colors
</commit_message>
<xml_diff>
--- a/data/MSCI-test-monthly.xlsx
+++ b/data/MSCI-test-monthly.xlsx
@@ -1300,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A266" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F280" activeCellId="0" sqref="F280"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F315" activeCellId="0" sqref="F315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1611,9 +1611,6 @@
       <c r="B25" s="1" t="n">
         <v>3198.647437</v>
       </c>
-      <c r="D25" s="1" t="n">
-        <v>582.187506</v>
-      </c>
       <c r="H25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,9 +1620,6 @@
       <c r="B26" s="1" t="n">
         <v>3249.513038</v>
       </c>
-      <c r="D26" s="1" t="n">
-        <v>594.627662</v>
-      </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,9 +1629,6 @@
       <c r="B27" s="1" t="n">
         <v>3312.625898</v>
       </c>
-      <c r="D27" s="1" t="n">
-        <v>611.751875</v>
-      </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,9 +1638,6 @@
       <c r="B28" s="1" t="n">
         <v>3033.040276</v>
       </c>
-      <c r="D28" s="1" t="n">
-        <v>559.16477</v>
-      </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,9 +1647,6 @@
       <c r="B29" s="1" t="n">
         <v>2834.396792</v>
       </c>
-      <c r="D29" s="1" t="n">
-        <v>519.295738</v>
-      </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,9 +1656,6 @@
       <c r="B30" s="1" t="n">
         <v>3044.611002</v>
       </c>
-      <c r="D30" s="1" t="n">
-        <v>558.590707</v>
-      </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,9 +1665,6 @@
       <c r="B31" s="1" t="n">
         <v>3006.795751</v>
       </c>
-      <c r="D31" s="1" t="n">
-        <v>554.666468</v>
-      </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,9 +1674,6 @@
       <c r="B32" s="1" t="n">
         <v>2913.015779</v>
       </c>
-      <c r="D32" s="1" t="n">
-        <v>539.642839</v>
-      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,9 +1683,6 @@
       <c r="B33" s="1" t="n">
         <v>2874.656129</v>
       </c>
-      <c r="D33" s="1" t="n">
-        <v>526.855609</v>
-      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,9 +1692,6 @@
       <c r="B34" s="1" t="n">
         <v>2737.232738</v>
       </c>
-      <c r="D34" s="1" t="n">
-        <v>504.70319</v>
-      </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,9 +1701,6 @@
       <c r="B35" s="1" t="n">
         <v>2496.400504</v>
       </c>
-      <c r="D35" s="1" t="n">
-        <v>455.014964</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -2238,9 +2205,6 @@
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="1" t="n">
-        <v>3076.904211</v>
-      </c>
       <c r="C72" s="1" t="n">
         <v>367.976153</v>
       </c>
@@ -2252,9 +2216,6 @@
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="1" t="n">
-        <v>3239.895069</v>
-      </c>
       <c r="C73" s="1" t="n">
         <v>388.188705</v>
       </c>
@@ -2266,9 +2227,6 @@
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="1" t="n">
-        <v>3364.558345</v>
-      </c>
       <c r="C74" s="1" t="n">
         <v>403.319699</v>
       </c>
@@ -2280,9 +2238,6 @@
       <c r="A75" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="1" t="n">
-        <v>3289.438908</v>
-      </c>
       <c r="C75" s="1" t="n">
         <v>394.851423</v>
       </c>
@@ -2294,9 +2249,6 @@
       <c r="A76" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="1" t="n">
-        <v>3395.133482</v>
-      </c>
       <c r="C76" s="1" t="n">
         <v>408.714016</v>
       </c>
@@ -2308,9 +2260,6 @@
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B77" s="1" t="n">
-        <v>3330.63462</v>
-      </c>
       <c r="C77" s="1" t="n">
         <v>399.871872</v>
       </c>
@@ -2322,9 +2271,6 @@
       <c r="A78" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="1" t="n">
-        <v>3260.390162</v>
-      </c>
       <c r="C78" s="1" t="n">
         <v>391.318985</v>
       </c>
@@ -2336,9 +2282,6 @@
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="1" t="n">
-        <v>3320.818075</v>
-      </c>
       <c r="C79" s="1" t="n">
         <v>398.919371</v>
       </c>
@@ -2350,9 +2293,6 @@
       <c r="A80" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="1" t="n">
-        <v>3351.01918</v>
-      </c>
       <c r="C80" s="1" t="n">
         <v>403.128063</v>
       </c>
@@ -2364,9 +2304,6 @@
       <c r="A81" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="1" t="n">
-        <v>3468.822784</v>
-      </c>
       <c r="C81" s="1" t="n">
         <v>418.142214</v>
       </c>
@@ -2378,9 +2315,6 @@
       <c r="A82" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B82" s="1" t="n">
-        <v>3496.581253</v>
-      </c>
       <c r="C82" s="1" t="n">
         <v>421.511812</v>
       </c>
@@ -2392,9 +2326,6 @@
       <c r="A83" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B83" s="1" t="n">
-        <v>3588.40956</v>
-      </c>
       <c r="C83" s="1" t="n">
         <v>434.311976</v>
       </c>
@@ -2406,9 +2337,6 @@
       <c r="A84" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B84" s="1" t="n">
-        <v>3502.062889</v>
-      </c>
       <c r="C84" s="1" t="n">
         <v>422.694633</v>
       </c>
@@ -2420,9 +2348,6 @@
       <c r="A85" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B85" s="1" t="n">
-        <v>3620.657193</v>
-      </c>
       <c r="C85" s="1" t="n">
         <v>438.304159</v>
       </c>
@@ -2434,9 +2359,6 @@
       <c r="A86" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B86" s="1" t="n">
-        <v>3701.794585</v>
-      </c>
       <c r="C86" s="1" t="n">
         <v>449.191746</v>
       </c>
@@ -2448,9 +2370,6 @@
       <c r="A87" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="1" t="n">
-        <v>3867.81377</v>
-      </c>
       <c r="C87" s="1" t="n">
         <v>471.403944</v>
       </c>
@@ -3134,9 +3053,6 @@
       <c r="A136" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B136" s="1" t="n">
-        <v>3714.830292</v>
-      </c>
       <c r="C136" s="1" t="n">
         <v>467.551022</v>
       </c>
@@ -3148,9 +3064,6 @@
       <c r="A137" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B137" s="1" t="n">
-        <v>3946.960009</v>
-      </c>
       <c r="C137" s="1" t="n">
         <v>497.859783</v>
       </c>
@@ -3162,79 +3075,46 @@
       <c r="A138" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B138" s="1" t="n">
-        <v>3949.717839</v>
-      </c>
       <c r="C138" s="1" t="n">
         <v>498.957126</v>
-      </c>
-      <c r="D138" s="1" t="n">
-        <v>837.18148</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B139" s="1" t="n">
-        <v>3575.136513</v>
-      </c>
       <c r="C139" s="1" t="n">
         <v>452.091868</v>
-      </c>
-      <c r="D139" s="1" t="n">
-        <v>758.253559</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B140" s="1" t="n">
-        <v>3453.891084</v>
-      </c>
       <c r="C140" s="1" t="n">
         <v>438.323072</v>
-      </c>
-      <c r="D140" s="1" t="n">
-        <v>734.311136</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B141" s="1" t="n">
-        <v>3734.815772</v>
-      </c>
       <c r="C141" s="1" t="n">
         <v>474.127677</v>
-      </c>
-      <c r="D141" s="1" t="n">
-        <v>793.856197</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B142" s="1" t="n">
-        <v>3596.902173</v>
-      </c>
       <c r="C142" s="1" t="n">
         <v>457.742383</v>
-      </c>
-      <c r="D142" s="1" t="n">
-        <v>765.897961</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B143" s="1" t="n">
-        <v>3933.681227</v>
-      </c>
       <c r="C143" s="1" t="n">
         <v>501.694253</v>
       </c>
@@ -3868,9 +3748,6 @@
       <c r="C188" s="1" t="n">
         <v>780.82468</v>
       </c>
-      <c r="D188" s="1" t="n">
-        <v>1320.041718</v>
-      </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
@@ -3882,9 +3759,6 @@
       <c r="C189" s="1" t="n">
         <v>771.590574</v>
       </c>
-      <c r="D189" s="1" t="n">
-        <v>1300.150424</v>
-      </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
@@ -3896,9 +3770,6 @@
       <c r="C190" s="1" t="n">
         <v>788.951765</v>
       </c>
-      <c r="D190" s="1" t="n">
-        <v>1330.786396</v>
-      </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
@@ -3910,9 +3781,6 @@
       <c r="C191" s="1" t="n">
         <v>763.672282</v>
       </c>
-      <c r="D191" s="1" t="n">
-        <v>1284.10162</v>
-      </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
@@ -3924,9 +3792,6 @@
       <c r="C192" s="1" t="n">
         <v>769.222984</v>
       </c>
-      <c r="D192" s="1" t="n">
-        <v>1294.501126</v>
-      </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
@@ -3938,9 +3803,6 @@
       <c r="C193" s="1" t="n">
         <v>782.418798</v>
       </c>
-      <c r="D193" s="1" t="n">
-        <v>1314.200392</v>
-      </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
@@ -3952,9 +3814,6 @@
       <c r="C194" s="1" t="n">
         <v>767.647049</v>
       </c>
-      <c r="D194" s="1" t="n">
-        <v>1293.084716</v>
-      </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
@@ -3966,9 +3825,6 @@
       <c r="C195" s="1" t="n">
         <v>755.816684</v>
       </c>
-      <c r="D195" s="1" t="n">
-        <v>1273.290271</v>
-      </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
@@ -3980,9 +3836,6 @@
       <c r="C196" s="1" t="n">
         <v>798.239834</v>
       </c>
-      <c r="D196" s="1" t="n">
-        <v>1345.0443</v>
-      </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
@@ -4982,9 +4835,6 @@
       <c r="A268" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B268" s="1" t="n">
-        <v>11811.310416</v>
-      </c>
       <c r="C268" s="1" t="n">
         <v>1406.021371</v>
       </c>
@@ -4996,9 +4846,6 @@
       <c r="A269" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B269" s="1" t="n">
-        <v>12211.116272</v>
-      </c>
       <c r="C269" s="1" t="n">
         <v>1444.322426</v>
       </c>
@@ -5010,9 +4857,6 @@
       <c r="A270" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B270" s="1" t="n">
-        <v>12784.973299</v>
-      </c>
       <c r="C270" s="1" t="n">
         <v>1508.067951</v>
       </c>
@@ -5024,9 +4868,6 @@
       <c r="A271" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B271" s="1" t="n">
-        <v>12976.577906</v>
-      </c>
       <c r="C271" s="1" t="n">
         <v>1532.347996</v>
       </c>
@@ -5038,9 +4879,6 @@
       <c r="A272" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B272" s="1" t="n">
-        <v>13174.250989</v>
-      </c>
       <c r="C272" s="1" t="n">
         <v>1553.044934</v>
       </c>
@@ -5052,9 +4890,6 @@
       <c r="A273" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B273" s="1" t="n">
-        <v>13413.449833</v>
-      </c>
       <c r="C273" s="1" t="n">
         <v>1564.196162</v>
       </c>
@@ -5072,9 +4907,6 @@
       <c r="C274" s="1" t="n">
         <v>1603.834282</v>
       </c>
-      <c r="D274" s="1" t="n">
-        <v>2694.235478</v>
-      </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
@@ -5086,9 +4918,6 @@
       <c r="C275" s="1" t="n">
         <v>1538.267293</v>
       </c>
-      <c r="D275" s="1" t="n">
-        <v>2587.973989</v>
-      </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
@@ -5100,9 +4929,6 @@
       <c r="C276" s="1" t="n">
         <v>1617.179623</v>
       </c>
-      <c r="D276" s="1" t="n">
-        <v>2714.524014</v>
-      </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
@@ -5114,9 +4940,6 @@
       <c r="C277" s="1" t="n">
         <v>1578.72871</v>
       </c>
-      <c r="D277" s="1" t="n">
-        <v>2642.472975</v>
-      </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
@@ -5128,9 +4951,6 @@
       <c r="C278" s="1" t="n">
         <v>1642.384553</v>
       </c>
-      <c r="D278" s="1" t="n">
-        <v>2748.266994</v>
-      </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
@@ -5142,9 +4962,6 @@
       <c r="C279" s="1" t="n">
         <v>1562.030228</v>
       </c>
-      <c r="D279" s="1" t="n">
-        <v>2606.15055</v>
-      </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
@@ -5390,9 +5207,6 @@
       <c r="A301" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B301" s="1" t="n">
-        <v>13871.961001</v>
-      </c>
       <c r="D301" s="1" t="n">
         <v>2615.355825</v>
       </c>
@@ -5401,9 +5215,6 @@
       <c r="A302" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B302" s="1" t="n">
-        <v>14557.826422</v>
-      </c>
       <c r="D302" s="1" t="n">
         <v>2753.489562</v>
       </c>
@@ -5412,9 +5223,6 @@
       <c r="A303" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B303" s="1" t="n">
-        <v>14735.888914</v>
-      </c>
       <c r="D303" s="1" t="n">
         <v>2760.285276</v>
       </c>
@@ -5423,9 +5231,6 @@
       <c r="A304" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B304" s="1" t="n">
-        <v>15366.381971</v>
-      </c>
       <c r="D304" s="1" t="n">
         <v>2876.617573</v>
       </c>
@@ -5434,12 +5239,6 @@
       <c r="A305" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B305" s="1" t="n">
-        <v>15868.8896</v>
-      </c>
-      <c r="D305" s="1" t="n">
-        <v>2969.190277</v>
-      </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
@@ -5448,9 +5247,6 @@
       <c r="B306" s="1" t="n">
         <v>15286.59151</v>
       </c>
-      <c r="D306" s="1" t="n">
-        <v>2869.658728</v>
-      </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
@@ -5459,9 +5255,6 @@
       <c r="B307" s="1" t="n">
         <v>15979.455491</v>
       </c>
-      <c r="D307" s="1" t="n">
-        <v>2987.735697</v>
-      </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
@@ -5470,9 +5263,6 @@
       <c r="B308" s="1" t="n">
         <v>16309.886618</v>
       </c>
-      <c r="D308" s="1" t="n">
-        <v>3044.186119</v>
-      </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
@@ -5481,9 +5271,6 @@
       <c r="B309" s="1" t="n">
         <v>16601.012475</v>
       </c>
-      <c r="D309" s="1" t="n">
-        <v>3107.654519</v>
-      </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
@@ -5492,9 +5279,6 @@
       <c r="B310" s="1" t="n">
         <v>17045.470265</v>
       </c>
-      <c r="D310" s="1" t="n">
-        <v>3181.292958</v>
-      </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
@@ -5503,9 +5287,6 @@
       <c r="B311" s="1" t="n">
         <v>17364.011736</v>
       </c>
-      <c r="D311" s="1" t="n">
-        <v>3255.7756</v>
-      </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
@@ -5514,9 +5295,6 @@
       <c r="B312" s="1" t="n">
         <v>17023.445476</v>
       </c>
-      <c r="D312" s="1" t="n">
-        <v>3181.390406</v>
-      </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
@@ -5525,9 +5303,6 @@
       <c r="B313" s="1" t="n">
         <v>17810.63517</v>
       </c>
-      <c r="D313" s="1" t="n">
-        <v>3306.465261</v>
-      </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
@@ -5536,9 +5311,6 @@
       <c r="B314" s="1" t="n">
         <v>17352.115351</v>
       </c>
-      <c r="D314" s="1" t="n">
-        <v>3218.643567</v>
-      </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
@@ -5547,9 +5319,6 @@
       <c r="B315" s="1" t="n">
         <v>17968.349835</v>
       </c>
-      <c r="D315" s="1" t="n">
-        <v>3324.731672</v>
-      </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
@@ -5558,9 +5327,6 @@
       <c r="B316" s="1" t="n">
         <v>17844.251038</v>
       </c>
-      <c r="D316" s="1" t="n">
-        <v>3296.400292</v>
-      </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
@@ -5569,9 +5335,6 @@
       <c r="B317" s="1" t="n">
         <v>17059.748793</v>
       </c>
-      <c r="D317" s="1" t="n">
-        <v>3170.354511</v>
-      </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
@@ -5580,9 +5343,6 @@
       <c r="B318" s="1" t="n">
         <v>17219.319838</v>
       </c>
-      <c r="D318" s="1" t="n">
-        <v>3201.495285</v>
-      </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
@@ -5591,9 +5351,6 @@
       <c r="B319" s="1" t="n">
         <v>18250.358313</v>
       </c>
-      <c r="D319" s="1" t="n">
-        <v>3388.827013</v>
-      </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
@@ -5602,9 +5359,6 @@
       <c r="B320" s="1" t="n">
         <v>19044.007434</v>
       </c>
-      <c r="D320" s="1" t="n">
-        <v>3543.895587</v>
-      </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
@@ -5612,9 +5366,6 @@
       </c>
       <c r="B321" s="1" t="n">
         <v>19293.050929</v>
-      </c>
-      <c r="D321" s="1" t="n">
-        <v>3591.95791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(data): print fill info only for missing columns
Reduce output clutter by printing missing value filling information only
for columns that actually have missing data. Other columns are processed
silently.
</commit_message>
<xml_diff>
--- a/data/MSCI-test-monthly.xlsx
+++ b/data/MSCI-test-monthly.xlsx
@@ -1300,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F315" activeCellId="0" sqref="F315"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A286" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E313" activeCellId="0" sqref="E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1611,6 +1611,9 @@
       <c r="B25" s="1" t="n">
         <v>3198.647437</v>
       </c>
+      <c r="D25" s="1" t="n">
+        <v>629.341775</v>
+      </c>
       <c r="H25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,6 +1623,9 @@
       <c r="B26" s="1" t="n">
         <v>3249.513038</v>
       </c>
+      <c r="D26" s="1" t="n">
+        <v>630.341775</v>
+      </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,6 +1635,9 @@
       <c r="B27" s="1" t="n">
         <v>3312.625898</v>
       </c>
+      <c r="D27" s="1" t="n">
+        <v>631.341775</v>
+      </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,6 +1647,9 @@
       <c r="B28" s="1" t="n">
         <v>3033.040276</v>
       </c>
+      <c r="D28" s="1" t="n">
+        <v>632.341775</v>
+      </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,6 +1659,9 @@
       <c r="B29" s="1" t="n">
         <v>2834.396792</v>
       </c>
+      <c r="D29" s="1" t="n">
+        <v>633.341775</v>
+      </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,6 +1671,9 @@
       <c r="B30" s="1" t="n">
         <v>3044.611002</v>
       </c>
+      <c r="D30" s="1" t="n">
+        <v>634.341775</v>
+      </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,6 +1683,9 @@
       <c r="B31" s="1" t="n">
         <v>3006.795751</v>
       </c>
+      <c r="D31" s="1" t="n">
+        <v>635.341775</v>
+      </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,6 +1695,9 @@
       <c r="B32" s="1" t="n">
         <v>2913.015779</v>
       </c>
+      <c r="D32" s="1" t="n">
+        <v>636.341775</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,6 +1707,9 @@
       <c r="B33" s="1" t="n">
         <v>2874.656129</v>
       </c>
+      <c r="D33" s="1" t="n">
+        <v>637.341775</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,6 +1719,9 @@
       <c r="B34" s="1" t="n">
         <v>2737.232738</v>
       </c>
+      <c r="D34" s="1" t="n">
+        <v>638.341775</v>
+      </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,6 +1731,9 @@
       <c r="B35" s="1" t="n">
         <v>2496.400504</v>
       </c>
+      <c r="D35" s="1" t="n">
+        <v>639.341775</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -2205,6 +2238,9 @@
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="B72" s="1" t="n">
+        <v>3003.6955</v>
+      </c>
       <c r="C72" s="1" t="n">
         <v>367.976153</v>
       </c>
@@ -2216,6 +2252,9 @@
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="B73" s="1" t="n">
+        <v>3004.6955</v>
+      </c>
       <c r="C73" s="1" t="n">
         <v>388.188705</v>
       </c>
@@ -2227,6 +2266,9 @@
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B74" s="1" t="n">
+        <v>3005.6955</v>
+      </c>
       <c r="C74" s="1" t="n">
         <v>403.319699</v>
       </c>
@@ -2238,6 +2280,9 @@
       <c r="A75" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B75" s="1" t="n">
+        <v>3006.6955</v>
+      </c>
       <c r="C75" s="1" t="n">
         <v>394.851423</v>
       </c>
@@ -2249,6 +2294,9 @@
       <c r="A76" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B76" s="1" t="n">
+        <v>3007.6955</v>
+      </c>
       <c r="C76" s="1" t="n">
         <v>408.714016</v>
       </c>
@@ -2260,6 +2308,9 @@
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="B77" s="1" t="n">
+        <v>3008.6955</v>
+      </c>
       <c r="C77" s="1" t="n">
         <v>399.871872</v>
       </c>
@@ -2271,6 +2322,9 @@
       <c r="A78" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="B78" s="1" t="n">
+        <v>3009.6955</v>
+      </c>
       <c r="C78" s="1" t="n">
         <v>391.318985</v>
       </c>
@@ -2282,6 +2336,9 @@
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="B79" s="1" t="n">
+        <v>3010.6955</v>
+      </c>
       <c r="C79" s="1" t="n">
         <v>398.919371</v>
       </c>
@@ -2293,6 +2350,9 @@
       <c r="A80" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="B80" s="1" t="n">
+        <v>3011.6955</v>
+      </c>
       <c r="C80" s="1" t="n">
         <v>403.128063</v>
       </c>
@@ -2304,6 +2364,9 @@
       <c r="A81" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="B81" s="1" t="n">
+        <v>3012.6955</v>
+      </c>
       <c r="C81" s="1" t="n">
         <v>418.142214</v>
       </c>
@@ -2315,6 +2378,9 @@
       <c r="A82" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="B82" s="1" t="n">
+        <v>3013.6955</v>
+      </c>
       <c r="C82" s="1" t="n">
         <v>421.511812</v>
       </c>
@@ -2326,6 +2392,9 @@
       <c r="A83" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="B83" s="1" t="n">
+        <v>3014.6955</v>
+      </c>
       <c r="C83" s="1" t="n">
         <v>434.311976</v>
       </c>
@@ -2337,6 +2406,9 @@
       <c r="A84" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="B84" s="1" t="n">
+        <v>3015.6955</v>
+      </c>
       <c r="C84" s="1" t="n">
         <v>422.694633</v>
       </c>
@@ -2348,6 +2420,9 @@
       <c r="A85" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B85" s="1" t="n">
+        <v>3016.6955</v>
+      </c>
       <c r="C85" s="1" t="n">
         <v>438.304159</v>
       </c>
@@ -2359,6 +2434,9 @@
       <c r="A86" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="B86" s="1" t="n">
+        <v>3017.6955</v>
+      </c>
       <c r="C86" s="1" t="n">
         <v>449.191746</v>
       </c>
@@ -2370,6 +2448,9 @@
       <c r="A87" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="B87" s="1" t="n">
+        <v>3018.6955</v>
+      </c>
       <c r="C87" s="1" t="n">
         <v>471.403944</v>
       </c>
@@ -3053,6 +3134,9 @@
       <c r="A136" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="B136" s="1" t="n">
+        <v>3662.751978</v>
+      </c>
       <c r="C136" s="1" t="n">
         <v>467.551022</v>
       </c>
@@ -3064,6 +3148,9 @@
       <c r="A137" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="B137" s="1" t="n">
+        <v>3663.751978</v>
+      </c>
       <c r="C137" s="1" t="n">
         <v>497.859783</v>
       </c>
@@ -3075,46 +3162,79 @@
       <c r="A138" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="B138" s="1" t="n">
+        <v>3664.751978</v>
+      </c>
       <c r="C138" s="1" t="n">
         <v>498.957126</v>
+      </c>
+      <c r="D138" s="1" t="n">
+        <v>832.647786</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B139" s="1" t="n">
+        <v>3665.751978</v>
+      </c>
       <c r="C139" s="1" t="n">
         <v>452.091868</v>
+      </c>
+      <c r="D139" s="1" t="n">
+        <v>833.647786</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="B140" s="1" t="n">
+        <v>3666.751978</v>
+      </c>
       <c r="C140" s="1" t="n">
         <v>438.323072</v>
+      </c>
+      <c r="D140" s="1" t="n">
+        <v>834.647786</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="B141" s="1" t="n">
+        <v>3667.751978</v>
+      </c>
       <c r="C141" s="1" t="n">
         <v>474.127677</v>
+      </c>
+      <c r="D141" s="1" t="n">
+        <v>835.647786</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="B142" s="1" t="n">
+        <v>3668.751978</v>
+      </c>
       <c r="C142" s="1" t="n">
         <v>457.742383</v>
+      </c>
+      <c r="D142" s="1" t="n">
+        <v>836.647786</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="B143" s="1" t="n">
+        <v>3669.751978</v>
+      </c>
       <c r="C143" s="1" t="n">
         <v>501.694253</v>
       </c>
@@ -3748,6 +3868,9 @@
       <c r="C188" s="1" t="n">
         <v>780.82468</v>
       </c>
+      <c r="D188" s="1" t="n">
+        <v>1292.968789</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
@@ -3759,6 +3882,9 @@
       <c r="C189" s="1" t="n">
         <v>771.590574</v>
       </c>
+      <c r="D189" s="1" t="n">
+        <v>1293.968789</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
@@ -3770,6 +3896,9 @@
       <c r="C190" s="1" t="n">
         <v>788.951765</v>
       </c>
+      <c r="D190" s="1" t="n">
+        <v>1294.968789</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
@@ -3781,6 +3910,9 @@
       <c r="C191" s="1" t="n">
         <v>763.672282</v>
       </c>
+      <c r="D191" s="1" t="n">
+        <v>1295.968789</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
@@ -3792,6 +3924,9 @@
       <c r="C192" s="1" t="n">
         <v>769.222984</v>
       </c>
+      <c r="D192" s="1" t="n">
+        <v>1296.968789</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
@@ -3803,6 +3938,9 @@
       <c r="C193" s="1" t="n">
         <v>782.418798</v>
       </c>
+      <c r="D193" s="1" t="n">
+        <v>1297.968789</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
@@ -3814,6 +3952,9 @@
       <c r="C194" s="1" t="n">
         <v>767.647049</v>
       </c>
+      <c r="D194" s="1" t="n">
+        <v>1298.968789</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
@@ -3825,6 +3966,9 @@
       <c r="C195" s="1" t="n">
         <v>755.816684</v>
       </c>
+      <c r="D195" s="1" t="n">
+        <v>1299.968789</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
@@ -3836,6 +3980,9 @@
       <c r="C196" s="1" t="n">
         <v>798.239834</v>
       </c>
+      <c r="D196" s="1" t="n">
+        <v>1300.968789</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
@@ -4835,6 +4982,9 @@
       <c r="A268" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="B268" s="1" t="n">
+        <v>11513.425105</v>
+      </c>
       <c r="C268" s="1" t="n">
         <v>1406.021371</v>
       </c>
@@ -4846,6 +4996,9 @@
       <c r="A269" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="B269" s="1" t="n">
+        <v>11514.425105</v>
+      </c>
       <c r="C269" s="1" t="n">
         <v>1444.322426</v>
       </c>
@@ -4857,6 +5010,9 @@
       <c r="A270" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="B270" s="1" t="n">
+        <v>11515.425105</v>
+      </c>
       <c r="C270" s="1" t="n">
         <v>1508.067951</v>
       </c>
@@ -4868,6 +5024,9 @@
       <c r="A271" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="B271" s="1" t="n">
+        <v>11516.425105</v>
+      </c>
       <c r="C271" s="1" t="n">
         <v>1532.347996</v>
       </c>
@@ -4879,6 +5038,9 @@
       <c r="A272" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="B272" s="1" t="n">
+        <v>11517.425105</v>
+      </c>
       <c r="C272" s="1" t="n">
         <v>1553.044934</v>
       </c>
@@ -4890,6 +5052,9 @@
       <c r="A273" s="1" t="s">
         <v>279</v>
       </c>
+      <c r="B273" s="1" t="n">
+        <v>11518.425105</v>
+      </c>
       <c r="C273" s="1" t="n">
         <v>1564.196162</v>
       </c>
@@ -4907,6 +5072,9 @@
       <c r="C274" s="1" t="n">
         <v>1603.834282</v>
       </c>
+      <c r="D274" s="1" t="n">
+        <v>2629.354585</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
@@ -4918,6 +5086,9 @@
       <c r="C275" s="1" t="n">
         <v>1538.267293</v>
       </c>
+      <c r="D275" s="1" t="n">
+        <v>2630.354585</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
@@ -4929,6 +5100,9 @@
       <c r="C276" s="1" t="n">
         <v>1617.179623</v>
       </c>
+      <c r="D276" s="1" t="n">
+        <v>2631.354585</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
@@ -4940,6 +5114,9 @@
       <c r="C277" s="1" t="n">
         <v>1578.72871</v>
       </c>
+      <c r="D277" s="1" t="n">
+        <v>2632.354585</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
@@ -4951,6 +5128,9 @@
       <c r="C278" s="1" t="n">
         <v>1642.384553</v>
       </c>
+      <c r="D278" s="1" t="n">
+        <v>2633.354585</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
@@ -4962,6 +5142,9 @@
       <c r="C279" s="1" t="n">
         <v>1562.030228</v>
       </c>
+      <c r="D279" s="1" t="n">
+        <v>2634.354585</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
@@ -5207,6 +5390,9 @@
       <c r="A301" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="B301" s="1" t="n">
+        <v>12677.970282</v>
+      </c>
       <c r="D301" s="1" t="n">
         <v>2615.355825</v>
       </c>
@@ -5215,6 +5401,9 @@
       <c r="A302" s="1" t="s">
         <v>308</v>
       </c>
+      <c r="B302" s="1" t="n">
+        <v>12678.970282</v>
+      </c>
       <c r="D302" s="1" t="n">
         <v>2753.489562</v>
       </c>
@@ -5223,6 +5412,9 @@
       <c r="A303" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="B303" s="1" t="n">
+        <v>12679.970282</v>
+      </c>
       <c r="D303" s="1" t="n">
         <v>2760.285276</v>
       </c>
@@ -5231,6 +5423,9 @@
       <c r="A304" s="1" t="s">
         <v>310</v>
       </c>
+      <c r="B304" s="1" t="n">
+        <v>12680.970282</v>
+      </c>
       <c r="D304" s="1" t="n">
         <v>2876.617573</v>
       </c>
@@ -5239,6 +5434,12 @@
       <c r="A305" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="B305" s="1" t="n">
+        <v>12681.970282</v>
+      </c>
+      <c r="D305" s="1" t="n">
+        <v>2877.617573</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
@@ -5247,6 +5448,9 @@
       <c r="B306" s="1" t="n">
         <v>15286.59151</v>
       </c>
+      <c r="D306" s="1" t="n">
+        <v>2878.617573</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
@@ -5255,6 +5459,9 @@
       <c r="B307" s="1" t="n">
         <v>15979.455491</v>
       </c>
+      <c r="D307" s="1" t="n">
+        <v>2879.617573</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
@@ -5263,6 +5470,9 @@
       <c r="B308" s="1" t="n">
         <v>16309.886618</v>
       </c>
+      <c r="D308" s="1" t="n">
+        <v>2880.617573</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
@@ -5271,6 +5481,9 @@
       <c r="B309" s="1" t="n">
         <v>16601.012475</v>
       </c>
+      <c r="D309" s="1" t="n">
+        <v>2881.617573</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
@@ -5279,6 +5492,9 @@
       <c r="B310" s="1" t="n">
         <v>17045.470265</v>
       </c>
+      <c r="D310" s="1" t="n">
+        <v>2882.617573</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
@@ -5287,6 +5503,9 @@
       <c r="B311" s="1" t="n">
         <v>17364.011736</v>
       </c>
+      <c r="D311" s="1" t="n">
+        <v>2883.617573</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
@@ -5295,6 +5514,9 @@
       <c r="B312" s="1" t="n">
         <v>17023.445476</v>
       </c>
+      <c r="D312" s="1" t="n">
+        <v>2884.617573</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
@@ -5303,6 +5525,9 @@
       <c r="B313" s="1" t="n">
         <v>17810.63517</v>
       </c>
+      <c r="D313" s="1" t="n">
+        <v>2885.617573</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
@@ -5311,6 +5536,9 @@
       <c r="B314" s="1" t="n">
         <v>17352.115351</v>
       </c>
+      <c r="D314" s="1" t="n">
+        <v>2886.617573</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
@@ -5319,6 +5547,9 @@
       <c r="B315" s="1" t="n">
         <v>17968.349835</v>
       </c>
+      <c r="D315" s="1" t="n">
+        <v>2887.617573</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
@@ -5327,6 +5558,9 @@
       <c r="B316" s="1" t="n">
         <v>17844.251038</v>
       </c>
+      <c r="D316" s="1" t="n">
+        <v>2888.617573</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
@@ -5335,6 +5569,9 @@
       <c r="B317" s="1" t="n">
         <v>17059.748793</v>
       </c>
+      <c r="D317" s="1" t="n">
+        <v>2889.617573</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
@@ -5343,6 +5580,9 @@
       <c r="B318" s="1" t="n">
         <v>17219.319838</v>
       </c>
+      <c r="D318" s="1" t="n">
+        <v>2890.617573</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
@@ -5351,6 +5591,9 @@
       <c r="B319" s="1" t="n">
         <v>18250.358313</v>
       </c>
+      <c r="D319" s="1" t="n">
+        <v>2891.617573</v>
+      </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
@@ -5359,6 +5602,9 @@
       <c r="B320" s="1" t="n">
         <v>19044.007434</v>
       </c>
+      <c r="D320" s="1" t="n">
+        <v>2892.617573</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
@@ -5366,6 +5612,9 @@
       </c>
       <c r="B321" s="1" t="n">
         <v>19293.050929</v>
+      </c>
+      <c r="D321" s="1" t="n">
+        <v>2893.617573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>